<commit_message>
Updated Niloshima's session details
</commit_message>
<xml_diff>
--- a/assets/downloads/Agenda.xlsx
+++ b/assets/downloads/Agenda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\System Libraries\Amal\Documents\AzConf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B96565C-A33D-4E44-8F8E-6CC8ACCB997C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539E6F25-29CA-4A60-9BA9-75611D640219}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="456" windowWidth="23016" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="280">
   <si>
     <t>DAY1</t>
   </si>
@@ -180,12 +180,6 @@
     <t>Azure Arc is Microsoft’s hybrid and multi-cloud platform. It has three components – Arc enabled servers, Arc enabled Kubernetes clusters, and Arc enabled data services. Attend this session to learn everything about Azure Arc capabilities. From registering and managing VMs to Kubernetes clusters to scaling PostgreSQL Hyperscale, this session has it all.</t>
   </si>
   <si>
-    <t>Managing Microservices with Servicemesh</t>
-  </si>
-  <si>
-    <t>Swaminathan Vetri</t>
-  </si>
-  <si>
     <t>D02-OPS01</t>
   </si>
   <si>
@@ -579,15 +573,9 @@
     <t>Azure Data Platform offers various services for all data professionals (Data Scientist, DBA, Developers, etc.) We will know all these services in order to select the most convenient for our next project</t>
   </si>
   <si>
-    <t>Content Moderator - A State of Art Cognitive Service</t>
-  </si>
-  <si>
     <t>Niloshima Srivastava</t>
   </si>
   <si>
-    <t>In this session, I would like to explain the core concepts of Azure Cognitive Service Content Moderator API. It is going to be a hands-on session which will complete - 1. The Core Concepts (Why to moderate, Ways to Moderate, and the Content Moderator API)  2. What is Automated Image Moderation (Concept and Demo)   3. Job Operations &amp; Review Operations (Concepts and Demo)</t>
-  </si>
-  <si>
     <t>4:30 PM</t>
   </si>
   <si>
@@ -654,9 +642,6 @@
     <t>D02-DEV202</t>
   </si>
   <si>
-    <t>Getting started with microservices is easy. As you start building tens/hundreds of microservices is when you would notice things are going out of control. That's where Service mesh comes to the rescue. In this session, you will learn how service mesh can help with easy traffic management &amp; observability for your microservices. The session would cover specifically about SMI (Service Mesh Interface) and OSM - Open Service Mesh</t>
-  </si>
-  <si>
     <t>D02-DEV302</t>
   </si>
   <si>
@@ -877,6 +862,19 @@
   </si>
   <si>
     <t xml:space="preserve">Lets solve a business problem togather using python, pandas, sklearn &amp; matplotlib. In this session, We will- Learn to use Azure studio for solving ai/ml problems - Understand the process of using python libraries  - Developing models for a business problem - Identifying an algorithm - Using hyperparameters to tune the accuracy - Training and testing the model    </t>
+  </si>
+  <si>
+    <t>In this talk, I would like to cover the following - 
+•	An Introduction to ML.NET
+•	What Apache Spark offers for .NET Stack
+•	Add the intelligence with Cognitive Services
+•	Explore Azure ML</t>
+  </si>
+  <si>
+    <t>Exploring Machine Learning for .Net Developers</t>
+  </si>
+  <si>
+    <t>TBA</t>
   </si>
 </sst>
 </file>
@@ -1560,22 +1558,6 @@
   <dxfs count="13">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1715,25 +1697,41 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1750,17 +1748,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H67" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H67" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H67" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Day" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start Time" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="End Time" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Session Code" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Title" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Speaker" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Overview" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Tags" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Day" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start Time" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="End Time" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Session Code" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Title" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Speaker" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Overview" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Tags" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2065,84 +2063,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F1" sqref="E1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="92.140625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.109375" style="5"/>
+    <col min="2" max="2" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.109375" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>4</v>
@@ -2151,18 +2149,18 @@
         <v>5</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>34</v>
@@ -2174,28 +2172,28 @@
         <v>36</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2203,19 +2201,19 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="H6" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2223,19 +2221,19 @@
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="H7" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2252,74 +2250,74 @@
         <v>11</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="H9" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="H10" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="H11" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2327,19 +2325,19 @@
         <v>14</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="H12" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2347,19 +2345,19 @@
         <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="H13" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2367,25 +2365,25 @@
         <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H14" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>17</v>
@@ -2401,36 +2399,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="H16" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>12</v>
@@ -2439,33 +2437,33 @@
         <v>13</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="H18" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2473,19 +2471,19 @@
         <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="H19" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2493,19 +2491,19 @@
         <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="H20" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2513,28 +2511,28 @@
         <v>26</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="H21" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>21</v>
@@ -2546,50 +2544,50 @@
         <v>23</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="H23" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="H24" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2597,19 +2595,19 @@
         <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="H25" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2617,19 +2615,19 @@
         <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2643,77 +2641,77 @@
         <v>32</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="H28" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="H29" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="H30" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2721,19 +2719,19 @@
         <v>37</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="H31" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2741,19 +2739,19 @@
         <v>38</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="H32" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2761,25 +2759,25 @@
         <v>40</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>182</v>
+        <v>278</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>184</v>
+        <v>277</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>41</v>
@@ -2792,18 +2790,18 @@
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>45</v>
@@ -2821,264 +2819,264 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="H36" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="H38" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>49</v>
+        <v>279</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>50</v>
+        <v>279</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="10"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>19</v>
@@ -3091,262 +3089,262 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H50" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="8"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>27</v>
@@ -3355,122 +3353,122 @@
         <v>28</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>42</v>
@@ -3478,14 +3476,15 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>